<commit_message>
update to raw data
</commit_message>
<xml_diff>
--- a/results/frequencies.xlsx
+++ b/results/frequencies.xlsx
@@ -476,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>6.67</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="3">
@@ -492,7 +492,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="n">
-        <v>15</v>
+        <v>15.52</v>
       </c>
     </row>
     <row r="4">
@@ -505,10 +505,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" t="n">
-        <v>63.33</v>
+        <v>62.07</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>8.33</v>
+        <v>8.619999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -540,7 +540,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>6.67</v>
+        <v>6.9</v>
       </c>
     </row>
   </sheetData>
@@ -594,10 +594,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="n">
-        <v>41.67</v>
+        <v>41.38</v>
       </c>
     </row>
     <row r="3">
@@ -610,10 +610,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="n">
-        <v>58.33</v>
+        <v>58.62</v>
       </c>
     </row>
   </sheetData>
@@ -666,7 +666,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>5.17</v>
       </c>
     </row>
     <row r="3">
@@ -679,10 +679,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3" t="n">
-        <v>90</v>
+        <v>89.66</v>
       </c>
     </row>
     <row r="4">
@@ -698,7 +698,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>5.17</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +755,7 @@
         <v>45</v>
       </c>
       <c r="D2" t="n">
-        <v>75</v>
+        <v>77.59</v>
       </c>
     </row>
     <row r="3">
@@ -771,7 +771,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="n">
-        <v>25</v>
+        <v>25.86</v>
       </c>
     </row>
     <row r="4">
@@ -787,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="5">
@@ -803,7 +803,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>15</v>
+        <v>15.52</v>
       </c>
     </row>
     <row r="6">
@@ -819,7 +819,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>8.33</v>
+        <v>8.619999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -835,7 +835,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="8">
@@ -851,7 +851,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>5.17</v>
       </c>
     </row>
     <row r="9">
@@ -867,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>5.17</v>
       </c>
     </row>
     <row r="10">
@@ -883,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>3.33</v>
+        <v>3.45</v>
       </c>
     </row>
   </sheetData>
@@ -932,7 +932,7 @@
         <v>45</v>
       </c>
       <c r="C2" t="n">
-        <v>75</v>
+        <v>77.59</v>
       </c>
     </row>
     <row r="3">
@@ -945,7 +945,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>25</v>
+        <v>25.86</v>
       </c>
     </row>
     <row r="4">
@@ -958,7 +958,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>16.67</v>
+        <v>17.24</v>
       </c>
     </row>
     <row r="5">
@@ -971,7 +971,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>10.34</v>
       </c>
     </row>
     <row r="6">
@@ -984,7 +984,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>8.33</v>
+        <v>8.619999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -997,7 +997,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>5.17</v>
       </c>
     </row>
   </sheetData>
@@ -1050,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="3">
@@ -1063,10 +1063,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3" t="n">
-        <v>90</v>
+        <v>89.66</v>
       </c>
     </row>
     <row r="4">
@@ -1082,7 +1082,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>6.67</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="5">
@@ -1098,7 +1098,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
     </row>
   </sheetData>
@@ -1155,7 +1155,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="n">
-        <v>31.67</v>
+        <v>32.76</v>
       </c>
     </row>
     <row r="3">
@@ -1168,10 +1168,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" t="n">
-        <v>41.67</v>
+        <v>39.66</v>
       </c>
     </row>
     <row r="4">
@@ -1187,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>3.33</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="5">
@@ -1203,7 +1203,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>11.67</v>
+        <v>12.07</v>
       </c>
     </row>
     <row r="6">
@@ -1219,7 +1219,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>3.33</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="7">
@@ -1235,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="8">
@@ -1251,7 +1251,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>6.67</v>
+        <v>6.9</v>
       </c>
     </row>
   </sheetData>
@@ -1305,10 +1305,10 @@
         <v>-1</v>
       </c>
       <c r="C2" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" t="n">
-        <v>55</v>
+        <v>53.45</v>
       </c>
     </row>
     <row r="3">
@@ -1324,7 +1324,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="n">
-        <v>15</v>
+        <v>15.52</v>
       </c>
     </row>
     <row r="4">
@@ -1340,7 +1340,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>13.33</v>
+        <v>13.79</v>
       </c>
     </row>
     <row r="5">
@@ -1356,7 +1356,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>5</v>
+        <v>5.17</v>
       </c>
     </row>
     <row r="6">
@@ -1372,7 +1372,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="n">
-        <v>11.67</v>
+        <v>12.07</v>
       </c>
     </row>
   </sheetData>
@@ -1429,7 +1429,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>10.34</v>
       </c>
     </row>
     <row r="3">
@@ -1445,7 +1445,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>16.67</v>
+        <v>17.24</v>
       </c>
     </row>
     <row r="4">
@@ -1458,10 +1458,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" t="n">
-        <v>63.33</v>
+        <v>62.07</v>
       </c>
     </row>
     <row r="5">
@@ -1477,7 +1477,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>3.33</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="6">
@@ -1493,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="7">
@@ -1509,7 +1509,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>5.17</v>
       </c>
     </row>
   </sheetData>
@@ -1563,10 +1563,10 @@
         <v>-1</v>
       </c>
       <c r="C2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="n">
-        <v>23.33</v>
+        <v>22.41</v>
       </c>
     </row>
     <row r="3">
@@ -1579,10 +1579,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="n">
-        <v>63.33</v>
+        <v>63.79</v>
       </c>
     </row>
     <row r="4">
@@ -1598,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1.67</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="5">
@@ -1614,7 +1614,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>6.67</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="6">
@@ -1630,7 +1630,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>5.17</v>
       </c>
     </row>
   </sheetData>
@@ -1644,7 +1644,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1675,47 +1675,35 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="B2" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D2" t="n">
-        <v>3.33</v>
+        <v>63.79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D3" t="n">
-        <v>61.67</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>21</v>
-      </c>
-      <c r="D4" t="n">
-        <v>35</v>
+        <v>36.21</v>
       </c>
     </row>
   </sheetData>
@@ -1769,10 +1757,10 @@
         <v>-1</v>
       </c>
       <c r="C2" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" t="n">
-        <v>65</v>
+        <v>63.79</v>
       </c>
     </row>
     <row r="3">
@@ -1788,7 +1776,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>20</v>
+        <v>20.69</v>
       </c>
     </row>
     <row r="4">
@@ -1804,7 +1792,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="n">
-        <v>15</v>
+        <v>15.52</v>
       </c>
     </row>
   </sheetData>
@@ -1858,10 +1846,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" t="n">
-        <v>76.67</v>
+        <v>75.86</v>
       </c>
     </row>
     <row r="3">
@@ -1877,7 +1865,7 @@
         <v>14</v>
       </c>
       <c r="D3" t="n">
-        <v>23.33</v>
+        <v>24.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>